<commit_message>
Added time of completion
</commit_message>
<xml_diff>
--- a/Chat-Application-Blueprint.xlsx
+++ b/Chat-Application-Blueprint.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FRENLEY\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FRENLEY\Desktop\chat_application\chat_application\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D008E9EA-ED11-4DB5-8387-6B3650941B83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C4DD5B7-E982-4307-A110-EF3AF8488071}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D9A41D8D-0628-4A2C-812F-6681BFEC898A}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="39">
   <si>
     <t>Chat Application Blueprint</t>
   </si>
@@ -157,6 +157,29 @@
   </si>
   <si>
     <t>admin can activate/deactivate festive/seasonal templates to the users</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Time Of Completion</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : 24th April 2020</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -611,10 +634,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87D78FE9-A798-40F6-B70B-B4BDAFD2A52F}">
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -834,6 +857,11 @@
         <v>24</v>
       </c>
     </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B19" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>